<commit_message>
add integration test code
</commit_message>
<xml_diff>
--- a/src/test/java/testCases/order/OrderTestData.xlsx
+++ b/src/test/java/testCases/order/OrderTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romadonz/Documents/Zanuar/DANA/Hands On Project/DANA Pulsa/Automation Testing/DanaPulsaAutomationTest/src/test/java/testCases/order/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{443C4CEE-0F77-AB48-A6B8-DCC11148F4F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E32F26FC-FB10-A844-93BE-79270C2B7864}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" activeTab="3" xr2:uid="{0BFCFD56-4938-304E-8F8D-A74A800CA122}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{0BFCFD56-4938-304E-8F8D-A74A800CA122}"/>
   </bookViews>
   <sheets>
     <sheet name="Recent Phone Number" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="67">
   <si>
     <t>sessionId</t>
   </si>
@@ -218,16 +218,7 @@
     <t>Valid ID (no transaction)</t>
   </si>
   <si>
-    <t>unknown transaction</t>
-  </si>
-  <si>
     <t>Valid ID (with transaction)</t>
-  </si>
-  <si>
-    <t>unknown user</t>
-  </si>
-  <si>
-    <t>invalid request format</t>
   </si>
   <si>
     <t>Undefined transaction ID</t>
@@ -1209,14 +1200,14 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -1243,13 +1234,11 @@
       <c r="C2" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>60</v>
-      </c>
+      <c r="D2" s="7"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>1</v>
@@ -1261,7 +1250,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>29</v>
@@ -1270,24 +1259,24 @@
         <v>1</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="14" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>63</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>1</v>
@@ -1295,37 +1284,33 @@
       <c r="C6" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>60</v>
-      </c>
+      <c r="D6" s="9"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B7" s="14" t="s">
         <v>1</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="9" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B8" s="14" t="s">
         <v>1</v>
       </c>
       <c r="C8" s="9"/>
-      <c r="D8" s="9" t="s">
-        <v>60</v>
-      </c>
+      <c r="D8" s="9"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B9" s="14" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
update integration test code
</commit_message>
<xml_diff>
--- a/src/test/java/testCases/order/OrderTestData.xlsx
+++ b/src/test/java/testCases/order/OrderTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romadonz/Documents/Zanuar/DANA/Hands On Project/DANA Pulsa/Automation Testing/DanaPulsaAutomationTest/src/test/java/testCases/order/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E32F26FC-FB10-A844-93BE-79270C2B7864}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D9034AE-146E-1C4B-91C5-C2CC47736F3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{0BFCFD56-4938-304E-8F8D-A74A800CA122}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" activeTab="2" xr2:uid="{0BFCFD56-4938-304E-8F8D-A74A800CA122}"/>
   </bookViews>
   <sheets>
     <sheet name="Recent Phone Number" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="70">
   <si>
     <t>sessionId</t>
   </si>
@@ -237,6 +237,15 @@
   </si>
   <si>
     <t>Empty String session ID</t>
+  </si>
+  <si>
+    <t>"method":"WALLET","phoneNumber":"081252930398","catalog":{"id":13,"provider":{"id":2,"name":"Telkomsel","image":"https://res.cloudinary.com/alvark/image/upload/v1592209103/danapulsa/Telkomsel_Logo_eviigt_nbbrjv.png"},"value":15000,"price":15000},"status":"CANCELED"</t>
+  </si>
+  <si>
+    <t>"code":400,"message":"can't cancel completed transaction"</t>
+  </si>
+  <si>
+    <t>"code":404,"message":"unknown transaction"</t>
   </si>
 </sst>
 </file>
@@ -928,8 +937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE0473D3-0997-FE4E-ADC8-4218DC8CB6C9}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1199,15 +1208,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56ABFCD1-161D-0348-8400-65ECCA6EDFC5}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="242.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -1234,7 +1243,9 @@
       <c r="C2" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="7"/>
+      <c r="D2" s="7" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
@@ -1246,7 +1257,9 @@
       <c r="C3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="7"/>
+      <c r="D3" s="7" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
@@ -1284,7 +1297,9 @@
       <c r="C6" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="9"/>
+      <c r="D6" s="7" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
@@ -1306,7 +1321,9 @@
         <v>1</v>
       </c>
       <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
+      <c r="D8" s="9" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
@@ -1318,7 +1335,9 @@
       <c r="C9" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="9"/>
+      <c r="D9" s="9" t="s">
+        <v>68</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>